<commit_message>
fix readme and xls
</commit_message>
<xml_diff>
--- a/docs/cases-considerations.xlsx
+++ b/docs/cases-considerations.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\keytiles\public-repos\keytiles-swagger-codegen\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F19D38-70F3-461E-A692-2269159E03F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B290CED-7E95-499B-9CEE-5468FC2B2CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28365" yWindow="1230" windowWidth="28065" windowHeight="13365" xr2:uid="{9BEC447D-165C-44CA-8873-6ECE22AAD055}"/>
+    <workbookView xWindow="435" yWindow="1230" windowWidth="28065" windowHeight="13365" xr2:uid="{9BEC447D-165C-44CA-8873-6ECE22AAD055}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="current implementation" sheetId="1" r:id="rId1"/>
+    <sheet name="just warning" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -144,8 +145,118 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Attila Wind</author>
+  </authors>
+  <commentList>
+    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{155F8848-5CB2-4075-BD1F-FEF5E37674C6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Attila Wind:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+schema warn: mandatory AND having default value is contradicting
+see: https://swagger.io/docs/specification/describing-parameters, "Default Parameter Values"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{288E3A74-49A2-41F8-B195-64AD3A55FE8F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Attila Wind:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+schema warn: mandatory AND having default value is contradicting
+see: https://swagger.io/docs/specification/describing-parameters, "Default Parameter Values"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C16" authorId="0" shapeId="0" xr:uid="{E037ED8D-5004-4F2C-8B6A-E7C56B63F3A6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Attila Wind:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+schema warn: mandatory AND having default value is contradicting
+see: https://swagger.io/docs/specification/describing-parameters, "Default Parameter Values"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C17" authorId="0" shapeId="0" xr:uid="{C72D9637-C1B3-4D41-8760-F03AE9233220}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Attila Wind:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+schema warn: mandatory AND having default value is contradicting
+see: https://swagger.io/docs/specification/describing-parameters, "Default Parameter Values"</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="30">
   <si>
     <t>nullable</t>
   </si>
@@ -192,21 +303,12 @@
     <t>yes - null check</t>
   </si>
   <si>
-    <t>private = def</t>
-  </si>
-  <si>
-    <t>private = NULL</t>
-  </si>
-  <si>
     <t>public = NULL</t>
   </si>
   <si>
     <t>no - public</t>
   </si>
   <si>
-    <t>public = def</t>
-  </si>
-  <si>
     <t>why ctor?</t>
   </si>
   <si>
@@ -231,17 +333,26 @@
     <t>field is final</t>
   </si>
   <si>
-    <t>yes  (and user can NULL)</t>
-  </si>
-  <si>
     <t>ERROR!</t>
+  </si>
+  <si>
+    <t>yes  (and user can pass NULL)</t>
+  </si>
+  <si>
+    <t>WARNING!</t>
+  </si>
+  <si>
+    <t>private = &lt;def&gt;</t>
+  </si>
+  <si>
+    <t>public = &lt;def&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -305,6 +416,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -359,18 +491,19 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -695,7 +828,7 @@
   <dimension ref="B1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,23 +841,511 @@
     <col min="6" max="6" width="10.5703125" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
     <col min="8" max="8" width="39.5703125" customWidth="1"/>
-    <col min="9" max="9" width="23" customWidth="1"/>
-    <col min="10" max="10" width="40.7109375" customWidth="1"/>
-    <col min="11" max="11" width="22.5703125" customWidth="1"/>
+    <col min="9" max="9" width="27" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" customWidth="1"/>
     <col min="12" max="12" width="96.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="9" t="s">
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" t="s">
+        <v>24</v>
+      </c>
+      <c r="K11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" t="s">
+        <v>3</v>
+      </c>
+      <c r="I15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" t="s">
+        <v>24</v>
+      </c>
+      <c r="K15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F78691C4-2E42-4AEB-961A-7561153CEE9A}">
+  <dimension ref="B1:K22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="39.5703125" customWidth="1"/>
+    <col min="9" max="9" width="27" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="96.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
@@ -737,7 +1358,7 @@
         <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K1" t="s">
         <v>8</v>
@@ -757,7 +1378,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
@@ -766,7 +1387,7 @@
         <v>14</v>
       </c>
       <c r="J2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K2" t="s">
         <v>14</v>
@@ -786,13 +1407,13 @@
         <v>0</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I3" t="s">
         <v>9</v>
       </c>
       <c r="K3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
@@ -809,7 +1430,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="H4" t="s">
         <v>12</v>
@@ -835,13 +1456,13 @@
         <v>0</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="I5" t="s">
         <v>9</v>
       </c>
       <c r="K5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
@@ -867,7 +1488,7 @@
         <v>14</v>
       </c>
       <c r="J6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K6" t="s">
         <v>14</v>
@@ -889,41 +1510,41 @@
       <c r="G7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>28</v>
+      <c r="I7" t="s">
+        <v>26</v>
       </c>
       <c r="J7" t="s">
         <v>2</v>
       </c>
       <c r="K7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>0</v>
       </c>
-      <c r="C8" s="2">
-        <v>1</v>
-      </c>
-      <c r="D8" s="2">
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="6" t="s">
+      <c r="F8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6" t="s">
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -931,25 +1552,25 @@
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9" s="2">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2">
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
         <v>1</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10">
@@ -974,7 +1595,7 @@
         <v>14</v>
       </c>
       <c r="J10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K10" t="s">
         <v>10</v>
@@ -1000,10 +1621,10 @@
         <v>3</v>
       </c>
       <c r="I11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K11" t="s">
         <v>10</v>
@@ -1032,7 +1653,7 @@
         <v>14</v>
       </c>
       <c r="J12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K12" t="s">
         <v>10</v>
@@ -1058,10 +1679,10 @@
         <v>3</v>
       </c>
       <c r="I13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K13" t="s">
         <v>10</v>
@@ -1090,7 +1711,7 @@
         <v>14</v>
       </c>
       <c r="J14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K14" t="s">
         <v>10</v>
@@ -1116,10 +1737,10 @@
         <v>3</v>
       </c>
       <c r="I15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K15" t="s">
         <v>10</v>
@@ -1129,31 +1750,31 @@
       <c r="B16">
         <v>0</v>
       </c>
-      <c r="C16" s="2">
-        <v>1</v>
-      </c>
-      <c r="D16" s="2">
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
         <v>1</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
-      <c r="F16" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G16" s="8" t="s">
+      <c r="F16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="I16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J16" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="K16" s="6" t="s">
+      <c r="J16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K16" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1161,47 +1782,47 @@
       <c r="B17">
         <v>1</v>
       </c>
-      <c r="C17" s="2">
-        <v>1</v>
-      </c>
-      <c r="D17" s="2">
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
         <v>1</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
-      <c r="F17" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G17" s="8" t="s">
+      <c r="F17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I17" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="K17" s="6" t="s">
+      <c r="I17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K17" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>